<commit_message>
Update fleet_key, add code 820
</commit_message>
<xml_diff>
--- a/data-raw/fleet_key.xlsx
+++ b/data-raw/fleet_key.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NoBackup\rpkgs\ICimportr\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NoBackup\SLU-Aqua-diadromous\catchstat\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="74">
   <si>
     <t>metier</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Mjärdar</t>
+  </si>
+  <si>
+    <t>FPO Burar, tinor, mjärdar</t>
   </si>
 </sst>
 </file>
@@ -577,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,9 +1306,20 @@
         <v>825</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63">
+        <v>820</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D62"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>